<commit_message>
update environmental predictors table for manuscript
</commit_message>
<xml_diff>
--- a/data/envPredictors.xlsx
+++ b/data/envPredictors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Predictor</t>
   </si>
@@ -75,18 +75,12 @@
     <t>5 days</t>
   </si>
   <si>
-    <t>SST Variance</t>
-  </si>
-  <si>
     <t>sst_sd</t>
   </si>
   <si>
     <t>Standard deviation of temperature at 2 m</t>
   </si>
   <si>
-    <t>Food availability, front probability</t>
-  </si>
-  <si>
     <t>17 days</t>
   </si>
   <si>
@@ -102,9 +96,6 @@
     <t>Food abundance</t>
   </si>
   <si>
-    <t>3 days</t>
-  </si>
-  <si>
     <t>Sathyendranath, et al., 2020</t>
   </si>
   <si>
@@ -138,9 +129,6 @@
     <t>Local upwelling intensity</t>
   </si>
   <si>
-    <t>13 days</t>
-  </si>
-  <si>
     <t>1 degree latitude</t>
   </si>
   <si>
@@ -166,6 +154,33 @@
   </si>
   <si>
     <t>García-Reyes &amp; Sydeman, 2017</t>
+  </si>
+  <si>
+    <t>Variable*</t>
+  </si>
+  <si>
+    <t>SST Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>Krill sex</t>
+  </si>
+  <si>
+    <t>Sexual dimorphism</t>
+  </si>
+  <si>
+    <t>Food availability</t>
+  </si>
+  <si>
+    <t>27 days</t>
+  </si>
+  <si>
+    <t>9 days</t>
   </si>
 </sst>
 </file>
@@ -534,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -613,19 +628,19 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -636,94 +651,117 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G7" t="s">
         <v>37</v>
-      </c>
-      <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
         <v>42</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chl-a spatial res in table 1
</commit_message>
<xml_diff>
--- a/data/envPredictors.xlsx
+++ b/data/envPredictors.xlsx
@@ -54,9 +54,6 @@
     <t>Direct impact of temperature on body size</t>
   </si>
   <si>
-    <t>2 days</t>
-  </si>
-  <si>
     <t>10 km</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>García-Reyes &amp; Sydeman, 2017</t>
   </si>
   <si>
-    <t>Variable*</t>
-  </si>
-  <si>
     <t>SST Standard Deviation</t>
   </si>
   <si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>9 days</t>
+  </si>
+  <si>
+    <t>4 km*</t>
+  </si>
+  <si>
+    <t>10 days</t>
   </si>
 </sst>
 </file>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -594,174 +594,174 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
         <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
-        <v>31</v>
-      </c>
       <c r="G6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" t="s">
         <v>35</v>
       </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>